<commit_message>
add javafx, refactor FastExcxel
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Datum</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>blume2000 se</t>
-  </si>
-  <si>
-    <t>11428.0</t>
   </si>
   <si>
     <t>Gesammt:</t>
@@ -91,9 +88,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="true"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <dxfs count="0"/>
 </styleSheet>
@@ -126,6 +121,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>11428.0</v>
+      </c>
+    </row>
     <row r="4">
       <c r="A4" s="2" t="s">
         <v>3</v>
@@ -137,15 +143,24 @@
         <v>11428.0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="n">
-        <v>22856.0</v>
+      <c r="C5" s="2" t="n">
+        <v>11428.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="n">
+        <v>34284.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>